<commit_message>
(web) clean supplemental datasets' metadata
</commit_message>
<xml_diff>
--- a/supplementary_data/supplementary_data_9.xlsx
+++ b/supplementary_data/supplementary_data_9.xlsx
@@ -2,15 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\team\lapt3u\projects\side\viral_titer\manuscript\_nature_comm_med_version\reviews\_editorial_resubmission\share\proof_docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4BB422-7347-4D7C-9D1B-C5F95E4A518A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A18A8C0-1D54-46DD-AE3F-CADBBDDADDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="936" windowWidth="23232" windowHeight="8508" xr2:uid="{C4E15537-405C-462F-80C5-37A77819AB9C}"/>
+    <workbookView xWindow="2184" yWindow="624" windowWidth="19884" windowHeight="13776" xr2:uid="{C4E15537-405C-462F-80C5-37A77819AB9C}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -8656,6 +8651,7 @@
     <mergeCell ref="A2:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -28790,6 +28786,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -65974,6 +65971,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -66069,5 +66067,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>